<commit_message>
sample year in 3
</commit_message>
<xml_diff>
--- a/OutputData/CCHF/01_09/CCHF_chord3_table.xlsx
+++ b/OutputData/CCHF/01_09/CCHF_chord3_table.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -510,7 +510,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -539,7 +539,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -622,7 +622,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -651,7 +651,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -680,7 +680,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -709,7 +709,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -767,7 +767,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -796,7 +796,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -825,7 +825,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -883,7 +883,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -912,7 +912,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -970,7 +970,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -999,7 +999,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1976 - 1980</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1971 - 1975</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1956 - 1960</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -2280,7 +2280,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1991 - 1995</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -3055,7 +3055,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -3283,7 +3283,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -3544,7 +3544,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -3602,7 +3602,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1956 - 1960</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -3830,7 +3830,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3859,7 +3859,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>1956 - 1960</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -3996,7 +3996,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>1961 - 1965</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -4083,7 +4083,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E128" t="n">
@@ -4112,7 +4112,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -4369,7 +4369,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E138" t="n">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -4427,7 +4427,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -4456,7 +4456,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -4485,7 +4485,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -4514,7 +4514,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -4543,7 +4543,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -4597,7 +4597,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E146" t="n">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E147" t="n">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E148" t="n">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E150" t="n">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>1976 - 1980</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E151" t="n">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E152" t="n">
@@ -4821,7 +4821,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E154" t="n">
@@ -4850,7 +4850,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E155" t="n">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E157" t="n">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E158" t="n">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E159" t="n">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E160" t="n">
@@ -5020,7 +5020,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E161" t="n">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E162" t="n">
@@ -5103,7 +5103,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E164" t="n">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E165" t="n">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E167" t="n">
@@ -5219,7 +5219,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E168" t="n">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E169" t="n">
@@ -5277,7 +5277,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E171" t="n">
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -5364,7 +5364,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E174" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E175" t="n">
@@ -5451,7 +5451,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E176" t="n">
@@ -5480,7 +5480,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>1971 - 1975</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E179" t="n">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -5592,7 +5592,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -5679,7 +5679,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E184" t="n">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E185" t="n">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -5766,7 +5766,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E187" t="n">
@@ -5820,7 +5820,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E189" t="n">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -5878,7 +5878,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E191" t="n">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E192" t="n">
@@ -5936,7 +5936,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E193" t="n">
@@ -5965,7 +5965,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E194" t="n">
@@ -6019,7 +6019,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E196" t="n">
@@ -6048,7 +6048,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E197" t="n">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>1971 - 1975</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E202" t="n">
@@ -6210,7 +6210,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E203" t="n">
@@ -6239,7 +6239,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -6268,7 +6268,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E205" t="n">
@@ -6297,7 +6297,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E206" t="n">
@@ -6326,7 +6326,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -6355,7 +6355,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E208" t="n">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E209" t="n">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E210" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E211" t="n">
@@ -6585,7 +6585,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E218" t="n">
@@ -6610,7 +6610,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>1991 - 1995</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E219" t="n">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E220" t="n">
@@ -6660,7 +6660,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E221" t="n">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E222" t="n">
@@ -6710,7 +6710,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E223" t="n">
@@ -6735,7 +6735,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E224" t="n">
@@ -6760,7 +6760,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E225" t="n">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>1976 - 1980</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E227" t="n">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>1976 - 1980</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E228" t="n">
@@ -6856,7 +6856,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E229" t="n">
@@ -6902,7 +6902,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E231" t="n">
@@ -6927,7 +6927,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>1996 - 2000</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E232" t="n">
@@ -6994,7 +6994,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E235" t="n">
@@ -7082,7 +7082,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E239" t="n">
@@ -7128,7 +7128,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>1981 - 1985</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E241" t="n">
@@ -7174,7 +7174,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>1986 - 1990</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E243" t="n">
@@ -7199,7 +7199,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>1991 - 1995</t>
+          <t>1978 - 1999</t>
         </is>
       </c>
       <c r="E244" t="n">
@@ -7249,7 +7249,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E246" t="n">
@@ -7278,7 +7278,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E247" t="n">
@@ -7307,7 +7307,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E248" t="n">
@@ -7336,7 +7336,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E249" t="n">
@@ -7365,7 +7365,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>2021 - 2025</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E250" t="n">
@@ -7394,7 +7394,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E251" t="n">
@@ -7423,7 +7423,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E252" t="n">
@@ -7452,7 +7452,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>2016 - 2020</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E253" t="n">
@@ -7481,7 +7481,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E254" t="n">
@@ -7510,7 +7510,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E255" t="n">
@@ -7539,7 +7539,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E256" t="n">
@@ -7568,7 +7568,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E257" t="n">
@@ -7597,7 +7597,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E258" t="n">
@@ -7626,7 +7626,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E259" t="n">
@@ -7655,7 +7655,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E260" t="n">
@@ -7684,7 +7684,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E261" t="n">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>1961 - 1965</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E262" t="n">
@@ -7742,7 +7742,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>1971 - 1975</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E263" t="n">
@@ -7771,7 +7771,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E264" t="n">
@@ -7800,7 +7800,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E265" t="n">
@@ -7829,7 +7829,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E266" t="n">
@@ -7858,7 +7858,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E267" t="n">
@@ -7887,7 +7887,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>1966 - 1970</t>
+          <t>1956 - 1977</t>
         </is>
       </c>
       <c r="E268" t="n">
@@ -7916,7 +7916,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E269" t="n">
@@ -7945,7 +7945,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E270" t="n">
@@ -7974,7 +7974,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>2006 - 2010</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E271" t="n">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>2011 - 2015</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E272" t="n">
@@ -8032,7 +8032,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>2001 - 2005</t>
+          <t>2000 - 2022</t>
         </is>
       </c>
       <c r="E273" t="n">

</xml_diff>